<commit_message>
0.1.2.1 - Internal Code changes
- Fixed Unit ID's
- Changed the way how the unitsize gets gathered
- Adjusted the Maphack- drwing slightly
</commit_message>
<xml_diff>
--- a/AnotherSc2Hack/Docs/WoL Unit-ID's.xlsx
+++ b/AnotherSc2Hack/Docs/WoL Unit-ID's.xlsx
@@ -4,19 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="90" windowWidth="20115" windowHeight="8250"/>
+    <workbookView xWindow="600" yWindow="90" windowWidth="3975" windowHeight="5475"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$B$4:$D$147</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="150">
   <si>
     <t>WoL Unit- ID's (ver.: 1.5.4.24540)</t>
   </si>
@@ -79,6 +82,393 @@
   </si>
   <si>
     <t>Viking (FLY)</t>
+  </si>
+  <si>
+    <t>Armory</t>
+  </si>
+  <si>
+    <t>Auto- Turret</t>
+  </si>
+  <si>
+    <t>Rax</t>
+  </si>
+  <si>
+    <t>Rax Fly</t>
+  </si>
+  <si>
+    <t>Bunker</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>CC Fly</t>
+  </si>
+  <si>
+    <t>Ebay</t>
+  </si>
+  <si>
+    <t>Fax</t>
+  </si>
+  <si>
+    <t>Fax Fly</t>
+  </si>
+  <si>
+    <t>Fusion Core</t>
+  </si>
+  <si>
+    <t>Ghost Academy</t>
+  </si>
+  <si>
+    <t>Missle Turret</t>
+  </si>
+  <si>
+    <t>OC</t>
+  </si>
+  <si>
+    <t>OC Fly</t>
+  </si>
+  <si>
+    <t>Planetary</t>
+  </si>
+  <si>
+    <t>Reactor</t>
+  </si>
+  <si>
+    <t>Reactor + Rax</t>
+  </si>
+  <si>
+    <t>Reactor + Fax</t>
+  </si>
+  <si>
+    <t>Reactor + SP</t>
+  </si>
+  <si>
+    <t>Sensor Tower</t>
+  </si>
+  <si>
+    <t>Starport</t>
+  </si>
+  <si>
+    <t>Starport Fly</t>
+  </si>
+  <si>
+    <t>Supply Depot</t>
+  </si>
+  <si>
+    <t>Supply Depot Lowered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tech </t>
+  </si>
+  <si>
+    <t>Tech + Rax</t>
+  </si>
+  <si>
+    <t>Tech + Fax</t>
+  </si>
+  <si>
+    <t>Tech + SP</t>
+  </si>
+  <si>
+    <t>Refinery</t>
+  </si>
+  <si>
+    <t>Gas Geysir</t>
+  </si>
+  <si>
+    <t>Terran</t>
+  </si>
+  <si>
+    <t>Neutral</t>
+  </si>
+  <si>
+    <t>Archon</t>
+  </si>
+  <si>
+    <t>Carrier</t>
+  </si>
+  <si>
+    <t>Colossus</t>
+  </si>
+  <si>
+    <t>DT</t>
+  </si>
+  <si>
+    <t>HAT</t>
+  </si>
+  <si>
+    <t>Immortal</t>
+  </si>
+  <si>
+    <t>Mothership</t>
+  </si>
+  <si>
+    <t>Observer</t>
+  </si>
+  <si>
+    <t>Phoenix</t>
+  </si>
+  <si>
+    <t>Probe</t>
+  </si>
+  <si>
+    <t>Sentry</t>
+  </si>
+  <si>
+    <t>Stalker</t>
+  </si>
+  <si>
+    <t>Void Ray</t>
+  </si>
+  <si>
+    <t>Warp Prism Phaasing</t>
+  </si>
+  <si>
+    <t>Warp Prism Transport</t>
+  </si>
+  <si>
+    <t>Zealot</t>
+  </si>
+  <si>
+    <t>Interceptor</t>
+  </si>
+  <si>
+    <t>Cyber Core</t>
+  </si>
+  <si>
+    <t>Dark Shrine</t>
+  </si>
+  <si>
+    <t>Fleet Beacon</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>Forge</t>
+  </si>
+  <si>
+    <t>GateWay</t>
+  </si>
+  <si>
+    <t>Nexus</t>
+  </si>
+  <si>
+    <t>Cannon</t>
+  </si>
+  <si>
+    <t>Pylon</t>
+  </si>
+  <si>
+    <t>Robotics Bay</t>
+  </si>
+  <si>
+    <t>Robitics Facility</t>
+  </si>
+  <si>
+    <t>Stargate</t>
+  </si>
+  <si>
+    <t>Templar Archives</t>
+  </si>
+  <si>
+    <t>Twilight Council</t>
+  </si>
+  <si>
+    <t>Warp Gate</t>
+  </si>
+  <si>
+    <t>Assimilator</t>
+  </si>
+  <si>
+    <t>Protoss</t>
+  </si>
+  <si>
+    <t>Baneling nest</t>
+  </si>
+  <si>
+    <t>Creep Tumor</t>
+  </si>
+  <si>
+    <t>Evo Chamber</t>
+  </si>
+  <si>
+    <t>Greater Spire</t>
+  </si>
+  <si>
+    <t>Hatchery</t>
+  </si>
+  <si>
+    <t>Hive</t>
+  </si>
+  <si>
+    <t>Hydra Den</t>
+  </si>
+  <si>
+    <t>Infestation Pit</t>
+  </si>
+  <si>
+    <t>Lair</t>
+  </si>
+  <si>
+    <t>Nydus Network</t>
+  </si>
+  <si>
+    <t>Nydus Worm</t>
+  </si>
+  <si>
+    <t>Roach warran</t>
+  </si>
+  <si>
+    <t>Spawning Pool</t>
+  </si>
+  <si>
+    <t>Sine Crawler</t>
+  </si>
+  <si>
+    <t>Spine Crawler unrooted</t>
+  </si>
+  <si>
+    <t>Spire</t>
+  </si>
+  <si>
+    <t>Spore Crawler</t>
+  </si>
+  <si>
+    <t>Spore Crawler unrooted</t>
+  </si>
+  <si>
+    <t>Ultra Cavern</t>
+  </si>
+  <si>
+    <t>Extractor</t>
+  </si>
+  <si>
+    <t>Larva</t>
+  </si>
+  <si>
+    <t>Baneling</t>
+  </si>
+  <si>
+    <t>Baneling Burrow</t>
+  </si>
+  <si>
+    <t>Baneling Cocoon</t>
+  </si>
+  <si>
+    <t>Brood Lord</t>
+  </si>
+  <si>
+    <t>Broodlord - Broodling</t>
+  </si>
+  <si>
+    <t>Broodlord Cocoom</t>
+  </si>
+  <si>
+    <t>Broodlord Escord</t>
+  </si>
+  <si>
+    <t>Changeling</t>
+  </si>
+  <si>
+    <t>Changeling Marineshield</t>
+  </si>
+  <si>
+    <t>Changeling Marine</t>
+  </si>
+  <si>
+    <t>Changeling Zealot</t>
+  </si>
+  <si>
+    <t>Changeling Speedling</t>
+  </si>
+  <si>
+    <t>Changeling Zergling</t>
+  </si>
+  <si>
+    <t>Corruptor</t>
+  </si>
+  <si>
+    <t>Drone</t>
+  </si>
+  <si>
+    <t>Drone Burrow</t>
+  </si>
+  <si>
+    <t>Egg</t>
+  </si>
+  <si>
+    <t>Hydra</t>
+  </si>
+  <si>
+    <t>Hydra Burrow</t>
+  </si>
+  <si>
+    <t>Infested Swarm Egg</t>
+  </si>
+  <si>
+    <t>Infested Terran</t>
+  </si>
+  <si>
+    <t>Infestor</t>
+  </si>
+  <si>
+    <t>Infestor Burrow</t>
+  </si>
+  <si>
+    <t>Muta</t>
+  </si>
+  <si>
+    <t>Overlord</t>
+  </si>
+  <si>
+    <t>Overseer</t>
+  </si>
+  <si>
+    <t>Ovserseer Cocoon</t>
+  </si>
+  <si>
+    <t>Queen</t>
+  </si>
+  <si>
+    <t>Queen Burrow</t>
+  </si>
+  <si>
+    <t>Roach</t>
+  </si>
+  <si>
+    <t>Roach Burrow</t>
+  </si>
+  <si>
+    <t>Ultra</t>
+  </si>
+  <si>
+    <t>Ultra Burrow</t>
+  </si>
+  <si>
+    <t>Zergling</t>
+  </si>
+  <si>
+    <t>Zergling Burrow</t>
+  </si>
+  <si>
+    <t>Zerg</t>
+  </si>
+  <si>
+    <t>Mineral Patch</t>
+  </si>
+  <si>
+    <t>Rich Mineral Patch</t>
+  </si>
+  <si>
+    <t>Rich Geyser</t>
+  </si>
+  <si>
+    <t>Space Geyser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xel Nage </t>
   </si>
 </sst>
 </file>
@@ -420,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E21"/>
+  <dimension ref="B2:E147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="B118" sqref="B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,90 +848,1583 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>4</v>
+        <v>56</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>5</v>
+        <v>46</v>
+      </c>
+      <c r="C6">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>6</v>
+        <v>47</v>
+      </c>
+      <c r="C7">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>7</v>
+        <v>48</v>
+      </c>
+      <c r="C8">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>8</v>
+        <v>49</v>
+      </c>
+      <c r="C9">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>9</v>
+        <v>37</v>
+      </c>
+      <c r="C10">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>10</v>
+        <v>38</v>
+      </c>
+      <c r="C11">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>11</v>
+        <v>39</v>
+      </c>
+      <c r="C12">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>12</v>
+        <v>129</v>
+      </c>
+      <c r="C13">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>13</v>
+        <v>111</v>
+      </c>
+      <c r="C14">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>14</v>
+        <v>109</v>
+      </c>
+      <c r="C15">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16">
+        <v>39</v>
+      </c>
+      <c r="D16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>132</v>
+      </c>
+      <c r="C17">
+        <v>39</v>
+      </c>
+      <c r="D17" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>116</v>
+      </c>
+      <c r="C19">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20">
+        <v>42</v>
+      </c>
+      <c r="D20" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21">
+        <v>43</v>
+      </c>
+      <c r="D21" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22">
+        <v>44</v>
+      </c>
+      <c r="D22" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23">
+        <v>45</v>
+      </c>
+      <c r="D23" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24">
+        <v>46</v>
+      </c>
+      <c r="D24" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25">
+        <v>48</v>
+      </c>
+      <c r="D25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26">
+        <v>49</v>
+      </c>
+      <c r="D26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27">
+        <v>50</v>
+      </c>
+      <c r="D27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28">
+        <v>51</v>
+      </c>
+      <c r="D28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>52</v>
+      </c>
+      <c r="D29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30">
+        <v>53</v>
+      </c>
+      <c r="D30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31">
+        <v>54</v>
+      </c>
+      <c r="D31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32">
+        <v>55</v>
+      </c>
+      <c r="D32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <v>56</v>
+      </c>
+      <c r="D33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34">
+        <v>57</v>
+      </c>
+      <c r="D34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35">
+        <v>58</v>
+      </c>
+      <c r="D35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36">
+        <v>60</v>
+      </c>
+      <c r="D36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37">
+        <v>61</v>
+      </c>
+      <c r="D37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38">
+        <v>62</v>
+      </c>
+      <c r="D38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39">
+        <v>63</v>
+      </c>
+      <c r="D39" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40">
+        <v>64</v>
+      </c>
+      <c r="D40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41">
+        <v>65</v>
+      </c>
+      <c r="D41" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>20</v>
+      </c>
+      <c r="C42">
+        <v>66</v>
+      </c>
+      <c r="D42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>27</v>
+      </c>
+      <c r="C43">
+        <v>67</v>
+      </c>
+      <c r="D43" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44">
+        <v>73</v>
+      </c>
+      <c r="D44" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>30</v>
+      </c>
+      <c r="C45">
+        <v>74</v>
+      </c>
+      <c r="D45" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>43</v>
+      </c>
+      <c r="C46">
+        <v>75</v>
+      </c>
+      <c r="D46" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="C47">
+        <v>76</v>
+      </c>
+      <c r="D47" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48">
+        <v>77</v>
+      </c>
+      <c r="D48" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49">
+        <v>78</v>
+      </c>
+      <c r="D49" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50">
+        <v>79</v>
+      </c>
+      <c r="D50" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51">
+        <v>80</v>
+      </c>
+      <c r="D51" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52">
+        <v>81</v>
+      </c>
+      <c r="D52" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>8</v>
+      </c>
+      <c r="C53">
+        <v>82</v>
+      </c>
+      <c r="D53" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>20</v>
+      <c r="C54">
+        <v>83</v>
+      </c>
+      <c r="D54" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55">
+        <v>84</v>
+      </c>
+      <c r="D55" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56">
+        <v>85</v>
+      </c>
+      <c r="D56" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57">
+        <v>86</v>
+      </c>
+      <c r="D57" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>13</v>
+      </c>
+      <c r="C58">
+        <v>87</v>
+      </c>
+      <c r="D58" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59">
+        <v>88</v>
+      </c>
+      <c r="D59" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>77</v>
+      </c>
+      <c r="C60">
+        <v>90</v>
+      </c>
+      <c r="D60" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>79</v>
+      </c>
+      <c r="C61">
+        <v>91</v>
+      </c>
+      <c r="D61" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>86</v>
+      </c>
+      <c r="C62">
+        <v>92</v>
+      </c>
+      <c r="D62" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>76</v>
+      </c>
+      <c r="C63">
+        <v>93</v>
+      </c>
+      <c r="D63" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>75</v>
+      </c>
+      <c r="C64">
+        <v>94</v>
+      </c>
+      <c r="D64" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>73</v>
+      </c>
+      <c r="C65">
+        <v>95</v>
+      </c>
+      <c r="D65" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>84</v>
+      </c>
+      <c r="C66">
+        <v>96</v>
+      </c>
+      <c r="D66" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>78</v>
+      </c>
+      <c r="C67">
+        <v>97</v>
+      </c>
+      <c r="D67" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>82</v>
+      </c>
+      <c r="C68">
+        <v>98</v>
+      </c>
+      <c r="D68" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>83</v>
+      </c>
+      <c r="C69">
+        <v>99</v>
+      </c>
+      <c r="D69" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>72</v>
+      </c>
+      <c r="C70">
+        <v>100</v>
+      </c>
+      <c r="D70" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>80</v>
+      </c>
+      <c r="C71">
+        <v>101</v>
+      </c>
+      <c r="D71" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>81</v>
+      </c>
+      <c r="C72">
+        <v>102</v>
+      </c>
+      <c r="D72" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>71</v>
+      </c>
+      <c r="C73">
+        <v>103</v>
+      </c>
+      <c r="D73" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>69</v>
+      </c>
+      <c r="C74">
+        <v>104</v>
+      </c>
+      <c r="D74" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>65</v>
+      </c>
+      <c r="C75">
+        <v>105</v>
+      </c>
+      <c r="D75" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>58</v>
+      </c>
+      <c r="C76">
+        <v>106</v>
+      </c>
+      <c r="D76" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>57</v>
+      </c>
+      <c r="C77">
+        <v>107</v>
+      </c>
+      <c r="D77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>64</v>
+      </c>
+      <c r="C78">
+        <v>108</v>
+      </c>
+      <c r="D78" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>62</v>
+      </c>
+      <c r="C79">
+        <v>109</v>
+      </c>
+      <c r="D79" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>55</v>
+      </c>
+      <c r="C80">
+        <v>110</v>
+      </c>
+      <c r="D80" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>66</v>
+      </c>
+      <c r="C81">
+        <v>111</v>
+      </c>
+      <c r="D81" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>68</v>
+      </c>
+      <c r="C82">
+        <v>112</v>
+      </c>
+      <c r="D82" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>61</v>
+      </c>
+      <c r="C83">
+        <v>113</v>
+      </c>
+      <c r="D83" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>59</v>
+      </c>
+      <c r="C84">
+        <v>114</v>
+      </c>
+      <c r="D84" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>63</v>
+      </c>
+      <c r="C85">
+        <v>115</v>
+      </c>
+      <c r="D85" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>70</v>
+      </c>
+      <c r="C86">
+        <v>116</v>
+      </c>
+      <c r="D86" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>74</v>
+      </c>
+      <c r="C87">
+        <v>116</v>
+      </c>
+      <c r="D87" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>92</v>
+      </c>
+      <c r="C88">
+        <v>117</v>
+      </c>
+      <c r="D88" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>107</v>
+      </c>
+      <c r="C89">
+        <v>119</v>
+      </c>
+      <c r="D89" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>100</v>
+      </c>
+      <c r="C90">
+        <v>120</v>
+      </c>
+      <c r="D90" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>90</v>
+      </c>
+      <c r="C91">
+        <v>121</v>
+      </c>
+      <c r="D91" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>94</v>
+      </c>
+      <c r="C92">
+        <v>122</v>
+      </c>
+      <c r="D92" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>103</v>
+      </c>
+      <c r="C93">
+        <v>123</v>
+      </c>
+      <c r="D93" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>106</v>
+      </c>
+      <c r="C94">
+        <v>124</v>
+      </c>
+      <c r="D94" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>95</v>
+      </c>
+      <c r="C95">
+        <v>125</v>
+      </c>
+      <c r="D95" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>97</v>
+      </c>
+      <c r="C96">
+        <v>126</v>
+      </c>
+      <c r="D96" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>88</v>
+      </c>
+      <c r="C97">
+        <v>127</v>
+      </c>
+      <c r="D97" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>99</v>
+      </c>
+      <c r="C98">
+        <v>128</v>
+      </c>
+      <c r="D98" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>101</v>
+      </c>
+      <c r="C99">
+        <v>129</v>
+      </c>
+      <c r="D99" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>104</v>
+      </c>
+      <c r="C100">
+        <v>130</v>
+      </c>
+      <c r="D100" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>96</v>
+      </c>
+      <c r="C101">
+        <v>131</v>
+      </c>
+      <c r="D101" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>93</v>
+      </c>
+      <c r="C102">
+        <v>132</v>
+      </c>
+      <c r="D102" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>91</v>
+      </c>
+      <c r="C103">
+        <v>133</v>
+      </c>
+      <c r="D103" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>125</v>
+      </c>
+      <c r="C104">
+        <v>134</v>
+      </c>
+      <c r="D104" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>123</v>
+      </c>
+      <c r="C105">
+        <v>135</v>
+      </c>
+      <c r="D105" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>142</v>
+      </c>
+      <c r="C106">
+        <v>136</v>
+      </c>
+      <c r="D106" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>133</v>
+      </c>
+      <c r="C107">
+        <v>137</v>
+      </c>
+      <c r="D107" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>126</v>
+      </c>
+      <c r="C108">
+        <v>138</v>
+      </c>
+      <c r="D108" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>140</v>
+      </c>
+      <c r="C109">
+        <v>140</v>
+      </c>
+      <c r="D109" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>138</v>
+      </c>
+      <c r="C110">
+        <v>141</v>
+      </c>
+      <c r="D110" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>130</v>
+      </c>
+      <c r="C111">
+        <v>142</v>
+      </c>
+      <c r="D111" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>122</v>
+      </c>
+      <c r="C112">
+        <v>143</v>
+      </c>
+      <c r="D112" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>114</v>
+      </c>
+      <c r="C113">
+        <v>144</v>
+      </c>
+      <c r="D113" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>112</v>
+      </c>
+      <c r="C114">
+        <v>145</v>
+      </c>
+      <c r="D114" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>110</v>
+      </c>
+      <c r="C115">
+        <v>146</v>
+      </c>
+      <c r="D115" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
+        <v>124</v>
+      </c>
+      <c r="C116">
+        <v>147</v>
+      </c>
+      <c r="D116" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
+        <v>127</v>
+      </c>
+      <c r="C117">
+        <v>148</v>
+      </c>
+      <c r="D117" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
+        <v>139</v>
+      </c>
+      <c r="C118">
+        <v>149</v>
+      </c>
+      <c r="D118" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B119" t="s">
+        <v>143</v>
+      </c>
+      <c r="C119">
+        <v>150</v>
+      </c>
+      <c r="D119" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B120" t="s">
+        <v>129</v>
+      </c>
+      <c r="C120">
+        <v>151</v>
+      </c>
+      <c r="D120" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B121" t="s">
+        <v>137</v>
+      </c>
+      <c r="C121">
+        <v>156</v>
+      </c>
+      <c r="D121" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B122" t="s">
+        <v>136</v>
+      </c>
+      <c r="C122">
+        <v>157</v>
+      </c>
+      <c r="D122" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B123" t="s">
+        <v>131</v>
+      </c>
+      <c r="C123">
+        <v>158</v>
+      </c>
+      <c r="D123" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B124" t="s">
+        <v>135</v>
+      </c>
+      <c r="C124">
+        <v>159</v>
+      </c>
+      <c r="D124" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B125" t="s">
+        <v>134</v>
+      </c>
+      <c r="C125">
+        <v>160</v>
+      </c>
+      <c r="D125" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B126" t="s">
+        <v>36</v>
+      </c>
+      <c r="C126">
+        <v>161</v>
+      </c>
+      <c r="D126" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B127" t="s">
+        <v>141</v>
+      </c>
+      <c r="C127">
+        <v>162</v>
+      </c>
+      <c r="D127" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B128" t="s">
+        <v>34</v>
+      </c>
+      <c r="C128">
+        <v>163</v>
+      </c>
+      <c r="D128" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B129" t="s">
+        <v>85</v>
+      </c>
+      <c r="C129">
+        <v>164</v>
+      </c>
+      <c r="D129" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B130" t="s">
+        <v>35</v>
+      </c>
+      <c r="C130">
+        <v>165</v>
+      </c>
+      <c r="D130" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B131" t="s">
+        <v>67</v>
+      </c>
+      <c r="C131">
+        <v>167</v>
+      </c>
+      <c r="D131" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B132" t="s">
+        <v>89</v>
+      </c>
+      <c r="C132">
+        <v>168</v>
+      </c>
+      <c r="D132" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B133" t="s">
+        <v>102</v>
+      </c>
+      <c r="C133">
+        <v>169</v>
+      </c>
+      <c r="D133" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B134" t="s">
+        <v>105</v>
+      </c>
+      <c r="C134">
+        <v>170</v>
+      </c>
+      <c r="D134" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
+        <v>54</v>
+      </c>
+      <c r="C135">
+        <v>171</v>
+      </c>
+      <c r="D135" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B136" t="s">
+        <v>98</v>
+      </c>
+      <c r="C136">
+        <v>172</v>
+      </c>
+      <c r="D136" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B137" t="s">
+        <v>115</v>
+      </c>
+      <c r="C137">
+        <v>173</v>
+      </c>
+      <c r="D137" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>146</v>
+      </c>
+      <c r="C138">
+        <v>174</v>
+      </c>
+      <c r="D138" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
+        <v>149</v>
+      </c>
+      <c r="C139">
+        <v>176</v>
+      </c>
+      <c r="D139" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
+        <v>128</v>
+      </c>
+      <c r="C140">
+        <v>180</v>
+      </c>
+      <c r="D140" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B141" t="s">
+        <v>108</v>
+      </c>
+      <c r="C141">
+        <v>181</v>
+      </c>
+      <c r="D141" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B142" t="s">
+        <v>11</v>
+      </c>
+      <c r="C142">
+        <v>189</v>
+      </c>
+      <c r="D142" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B143" t="s">
+        <v>113</v>
+      </c>
+      <c r="C143">
+        <v>212</v>
+      </c>
+      <c r="D143" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B144" t="s">
+        <v>145</v>
+      </c>
+      <c r="C144">
+        <v>253</v>
+      </c>
+      <c r="D144" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="145" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B145" t="s">
+        <v>51</v>
+      </c>
+      <c r="C145">
+        <v>254</v>
+      </c>
+      <c r="D145" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="146" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B146" t="s">
+        <v>148</v>
+      </c>
+      <c r="C146">
+        <v>255</v>
+      </c>
+      <c r="D146" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="147" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B147" t="s">
+        <v>147</v>
+      </c>
+      <c r="C147">
+        <v>256</v>
+      </c>
+      <c r="D147" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B4:D147">
+    <sortState ref="B5:D147">
+      <sortCondition ref="C4:C147"/>
+    </sortState>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="B2:E3"/>
   </mergeCells>

</xml_diff>